<commit_message>
slot entry is ok
</commit_message>
<xml_diff>
--- a/AchainMysql.xlsx
+++ b/AchainMysql.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="225" tabRatio="844" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="225" tabRatio="844" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sort_out" sheetId="18" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="293">
   <si>
     <t>_block_extend_status</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -702,10 +702,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无数据，</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>total_paid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -754,10 +750,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>account_entry</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>titan_account</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -779,10 +771,6 @@
   </si>
   <si>
     <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1113,10 +1101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>call_contract_op_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>transfer_contract_op_type,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1146,6 +1130,18 @@
   </si>
   <si>
     <t>withdraw_balance_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account_entry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2104,7 +2100,7 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -2126,7 +2122,7 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
@@ -2137,13 +2133,13 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="30"/>
       <c r="B30" s="31" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C30" t="s">
         <v>157</v>
@@ -2206,7 +2202,7 @@
   <sheetData>
     <row r="1" spans="1:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -2253,7 +2249,7 @@
     </row>
     <row r="6" spans="1:4" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>84</v>
@@ -2273,7 +2269,7 @@
         <v>91</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4" customFormat="1" x14ac:dyDescent="0.15">
@@ -2314,7 +2310,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>93</v>
@@ -2362,14 +2358,14 @@
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>21</v>
@@ -2380,63 +2376,63 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="36"/>
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="36"/>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="40"/>
     </row>
     <row r="9" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2472,14 +2468,14 @@
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>21</v>
@@ -2490,7 +2486,7 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="8"/>
@@ -2504,7 +2500,7 @@
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="40"/>
@@ -2554,7 +2550,7 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
@@ -2563,7 +2559,7 @@
     </row>
     <row r="4" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
@@ -2632,8 +2628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2646,14 +2642,14 @@
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="56" t="s">
-        <v>185</v>
+        <v>291</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>21</v>
@@ -2664,7 +2660,7 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
@@ -2673,7 +2669,7 @@
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>192</v>
+        <v>290</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -2709,11 +2705,11 @@
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
@@ -2727,7 +2723,7 @@
     </row>
     <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="25" t="s">
@@ -2736,7 +2732,7 @@
     </row>
     <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="25" t="s">
@@ -2745,7 +2741,7 @@
     </row>
     <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
@@ -2754,7 +2750,7 @@
     </row>
     <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -2763,20 +2759,20 @@
     </row>
     <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>172</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2981,7 +2977,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3015,7 +3011,7 @@
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -3035,7 +3031,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3122,8 +3118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3150,167 +3146,167 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="41" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="41" t="s">
-        <v>287</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>289</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="41" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>291</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>286</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="12" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>288</v>
-      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="15" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>271</v>
+        <v>205</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>289</v>
-      </c>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3364,210 +3360,210 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C15" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C16" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C17" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C19" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C21" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C22" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C23" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C25" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C26" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all tables are ok
</commit_message>
<xml_diff>
--- a/AchainMysql.xlsx
+++ b/AchainMysql.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="225" tabRatio="844" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="225" tabRatio="844" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sort_out" sheetId="18" r:id="rId1"/>
@@ -750,10 +750,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>titan_account</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>账户地址</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1142,6 +1138,10 @@
   </si>
   <si>
     <t>无数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>titan_account</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2139,7 +2139,7 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="30"/>
       <c r="B30" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30" t="s">
         <v>157</v>
@@ -2202,7 +2202,7 @@
   <sheetData>
     <row r="1" spans="1:4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="6" spans="1:4" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>84</v>
@@ -2310,7 +2310,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>93</v>
@@ -2358,14 +2358,14 @@
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>21</v>
@@ -2376,63 +2376,63 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="36"/>
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="36"/>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="40"/>
     </row>
     <row r="9" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2468,14 +2468,14 @@
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>21</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="40"/>
@@ -2628,21 +2628,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.75" style="12" customWidth="1"/>
+    <col min="2" max="2" width="37.875" style="12" customWidth="1"/>
     <col min="3" max="3" width="24.5" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
@@ -2669,7 +2669,7 @@
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -2705,11 +2705,11 @@
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
@@ -2759,20 +2759,20 @@
     </row>
     <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>184</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2998,20 +2998,20 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="48.25" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3118,8 +3118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3146,50 +3146,50 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3203,110 +3203,110 @@
     </row>
     <row r="10" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3360,210 +3360,210 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>